<commit_message>
Added Design Expert files
</commit_message>
<xml_diff>
--- a/Model training and optimisations/Factorial Analysis - Membrane Model/Design.xlsx
+++ b/Model training and optimisations/Factorial Analysis - Membrane Model/Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://canonpp-my.sharepoint.com/personal/freek_klabbers_cpp_canon/Documents/Documents/GitHub/Predictive-Maintenance-Membrane-pumpm/Model training and optimisations/Factorial Analysis - Membrane Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{A22B7F2A-2D4E-4A42-863E-4816B5CC037A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{665ED528-C36E-489A-BCE2-5A3BC36826FE}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{A22B7F2A-2D4E-4A42-863E-4816B5CC037A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10886B86-109C-443C-BD55-64688DE96EBA}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2543DC8A-59FD-494E-8FB3-531C3EBE7859}"/>
   </bookViews>
@@ -450,7 +450,7 @@
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,13 +512,13 @@
         <v>3</v>
       </c>
       <c r="G2" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H2" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I2" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -541,13 +541,13 @@
         <v>3</v>
       </c>
       <c r="G3" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I3" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -570,13 +570,13 @@
         <v>3</v>
       </c>
       <c r="G4" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H4" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I4" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -599,13 +599,13 @@
         <v>3</v>
       </c>
       <c r="G5" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H5" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I5" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -625,16 +625,16 @@
         <v>-1</v>
       </c>
       <c r="F6" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G6" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H6" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I6" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -654,16 +654,16 @@
         <v>-1</v>
       </c>
       <c r="F7" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G7" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H7" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I7" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -683,16 +683,16 @@
         <v>-1</v>
       </c>
       <c r="F8" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G8" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H8" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I8" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -712,16 +712,16 @@
         <v>-1</v>
       </c>
       <c r="F9" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G9" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H9" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I9" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -744,13 +744,13 @@
         <v>3</v>
       </c>
       <c r="G10" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H10" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I10" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -773,13 +773,13 @@
         <v>3</v>
       </c>
       <c r="G11" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H11" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I11" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -802,13 +802,13 @@
         <v>3</v>
       </c>
       <c r="G12" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H12" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I12" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -831,13 +831,13 @@
         <v>3</v>
       </c>
       <c r="G13" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H13" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I13" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -857,16 +857,16 @@
         <v>-1</v>
       </c>
       <c r="F14" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G14" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H14" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I14" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -886,16 +886,16 @@
         <v>-1</v>
       </c>
       <c r="F15" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G15" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H15" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I15" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -915,16 +915,16 @@
         <v>-1</v>
       </c>
       <c r="F16" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G16" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H16" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I16" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -944,16 +944,16 @@
         <v>-1</v>
       </c>
       <c r="F17" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G17" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H17" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I17" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -976,13 +976,13 @@
         <v>3</v>
       </c>
       <c r="G18" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H18" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I18" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1005,13 +1005,13 @@
         <v>3</v>
       </c>
       <c r="G19" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H19" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I19" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1034,13 +1034,13 @@
         <v>3</v>
       </c>
       <c r="G20" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H20" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I20" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1063,13 +1063,13 @@
         <v>3</v>
       </c>
       <c r="G21" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H21" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I21" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1089,16 +1089,16 @@
         <v>-1</v>
       </c>
       <c r="F22" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G22" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H22" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I22" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1118,16 +1118,16 @@
         <v>-1</v>
       </c>
       <c r="F23" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G23" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H23" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I23" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1147,16 +1147,16 @@
         <v>-1</v>
       </c>
       <c r="F24" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G24" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H24" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I24" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1176,16 +1176,16 @@
         <v>-1</v>
       </c>
       <c r="F25" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G25" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H25" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I25" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1208,13 +1208,13 @@
         <v>3</v>
       </c>
       <c r="G26" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H26" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I26" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1237,13 +1237,13 @@
         <v>3</v>
       </c>
       <c r="G27" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H27" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I27" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1266,13 +1266,13 @@
         <v>3</v>
       </c>
       <c r="G28" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H28" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I28" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1295,13 +1295,13 @@
         <v>3</v>
       </c>
       <c r="G29" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H29" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I29" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1321,16 +1321,16 @@
         <v>-1</v>
       </c>
       <c r="F30" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G30" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H30" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I30" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1350,16 +1350,16 @@
         <v>-1</v>
       </c>
       <c r="F31" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G31" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H31" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I31" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1379,16 +1379,16 @@
         <v>-1</v>
       </c>
       <c r="F32" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G32" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H32" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I32" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1408,16 +1408,16 @@
         <v>-1</v>
       </c>
       <c r="F33" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G33" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H33" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I33" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1440,13 +1440,13 @@
         <v>3</v>
       </c>
       <c r="G34" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H34" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I34" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1469,13 +1469,13 @@
         <v>3</v>
       </c>
       <c r="G35" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H35" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I35" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1498,13 +1498,13 @@
         <v>3</v>
       </c>
       <c r="G36" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H36" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I36" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1527,13 +1527,13 @@
         <v>3</v>
       </c>
       <c r="G37" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H37" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I37" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1553,16 +1553,16 @@
         <v>1</v>
       </c>
       <c r="F38" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G38" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H38" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I38" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1582,16 +1582,16 @@
         <v>1</v>
       </c>
       <c r="F39" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G39" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H39" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I39" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1611,16 +1611,16 @@
         <v>1</v>
       </c>
       <c r="F40" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G40" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H40" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I40" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1640,16 +1640,16 @@
         <v>1</v>
       </c>
       <c r="F41" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G41" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H41" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I41" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1672,13 +1672,13 @@
         <v>3</v>
       </c>
       <c r="G42" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H42" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I42" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1701,13 +1701,13 @@
         <v>3</v>
       </c>
       <c r="G43" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H43" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I43" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -1730,13 +1730,13 @@
         <v>3</v>
       </c>
       <c r="G44" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H44" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I44" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -1759,13 +1759,13 @@
         <v>3</v>
       </c>
       <c r="G45" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H45" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I45" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -1785,16 +1785,16 @@
         <v>1</v>
       </c>
       <c r="F46" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G46" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H46" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I46" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -1814,16 +1814,16 @@
         <v>1</v>
       </c>
       <c r="F47" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G47" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H47" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I47" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -1843,16 +1843,16 @@
         <v>1</v>
       </c>
       <c r="F48" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G48" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H48" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I48" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -1872,16 +1872,16 @@
         <v>1</v>
       </c>
       <c r="F49" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G49" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H49" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I49" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -1904,13 +1904,13 @@
         <v>3</v>
       </c>
       <c r="G50" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H50" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I50" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -1933,13 +1933,13 @@
         <v>3</v>
       </c>
       <c r="G51" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H51" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I51" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -1962,13 +1962,13 @@
         <v>3</v>
       </c>
       <c r="G52" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H52" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I52" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -1991,13 +1991,13 @@
         <v>3</v>
       </c>
       <c r="G53" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H53" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I53" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2017,16 +2017,16 @@
         <v>1</v>
       </c>
       <c r="F54" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G54" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H54" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I54" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2046,16 +2046,16 @@
         <v>1</v>
       </c>
       <c r="F55" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G55" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H55" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I55" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2075,16 +2075,16 @@
         <v>1</v>
       </c>
       <c r="F56" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G56" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H56" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I56" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2104,16 +2104,16 @@
         <v>1</v>
       </c>
       <c r="F57" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G57" s="1">
-        <v>0.05</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="H57" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I57" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2136,13 +2136,13 @@
         <v>3</v>
       </c>
       <c r="G58" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H58" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I58" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2165,13 +2165,13 @@
         <v>3</v>
       </c>
       <c r="G59" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H59" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I59" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2194,13 +2194,13 @@
         <v>3</v>
       </c>
       <c r="G60" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H60" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I60" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2223,13 +2223,13 @@
         <v>3</v>
       </c>
       <c r="G61" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H61" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I61" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2249,16 +2249,16 @@
         <v>1</v>
       </c>
       <c r="F62" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G62" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H62" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I62" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2278,16 +2278,16 @@
         <v>1</v>
       </c>
       <c r="F63" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G63" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H63" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I63" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2307,16 +2307,16 @@
         <v>1</v>
       </c>
       <c r="F64" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G64" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H64" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I64" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2336,16 +2336,16 @@
         <v>1</v>
       </c>
       <c r="F65" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G65" s="1">
-        <v>9.9999999999999992E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H65" s="1">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I65" s="1">
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2365,16 +2365,16 @@
         <v>0</v>
       </c>
       <c r="F66" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G66" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H66" s="1">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="I66" s="1">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2394,16 +2394,16 @@
         <v>0</v>
       </c>
       <c r="F67" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G67" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H67" s="1">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="I67" s="1">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -2423,16 +2423,16 @@
         <v>0</v>
       </c>
       <c r="F68" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G68" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H68" s="1">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="I68" s="1">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -2452,16 +2452,16 @@
         <v>0</v>
       </c>
       <c r="F69" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G69" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H69" s="1">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="I69" s="1">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>